<commit_message>
Fix generating Excel schedule in horario.py
</commit_message>
<xml_diff>
--- a/static/schedule-instructores/Horario 1-2024 - DORIAN SULLY MÚNERA RÚA.xlsx
+++ b/static/schedule-instructores/Horario 1-2024 - DORIAN SULLY MÚNERA RÚA.xlsx
@@ -475,7 +475,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:G30"/>
+  <dimension ref="A2:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1007,70 +1007,215 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="6" t="inlineStr">
+      <c r="A29" s="6" t="inlineStr"/>
+      <c r="B29" s="6" t="inlineStr"/>
+      <c r="C29" s="6" t="inlineStr">
+        <is>
+          <t>MULTIMEDIA</t>
+        </is>
+      </c>
+      <c r="D29" s="6" t="inlineStr">
+        <is>
+          <t>Negociación, Marketing Digital</t>
+        </is>
+      </c>
+      <c r="E29" s="6" t="inlineStr">
+        <is>
+          <t>Realizar negociación con los proveedores y clientes, según los objetivos y estrategias establecidas por la organización.</t>
+        </is>
+      </c>
+      <c r="F29" s="6" t="inlineStr">
+        <is>
+          <t>Realizar negociación con los proveedores y clientes, según los objetivos y estrategias establecidas por la organización.</t>
+        </is>
+      </c>
+      <c r="G29" s="6" t="inlineStr">
+        <is>
+          <t>Crear la propuesta y/o contrapropuesta que establezca detalles de rentabilidad, precios, y compromisos con base en las políticas del cliente (financiación, presupuesto, objetivos e identidad corporativa). (Negociación – Marketing Digital)</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="6" t="inlineStr"/>
+      <c r="B30" s="6" t="inlineStr"/>
+      <c r="C30" s="6" t="inlineStr">
+        <is>
+          <t>MULTIMEDIA</t>
+        </is>
+      </c>
+      <c r="D30" s="6" t="inlineStr">
+        <is>
+          <t>Negociación, Marketing Digital</t>
+        </is>
+      </c>
+      <c r="E30" s="6" t="inlineStr">
+        <is>
+          <t>Realizar negociación con los proveedores y clientes, según los objetivos y estrategias establecidas por la organización.</t>
+        </is>
+      </c>
+      <c r="F30" s="6" t="inlineStr">
+        <is>
+          <t>Realizar negociación con los proveedores y clientes, según los objetivos y estrategias establecidas por la organización.</t>
+        </is>
+      </c>
+      <c r="G30" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Identificar las tendencias del mercado y del diseño en la producción de proyectos multimedia para orientar al cliente. </t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="inlineStr"/>
+      <c r="B31" s="6" t="inlineStr"/>
+      <c r="C31" s="6" t="inlineStr">
+        <is>
+          <t>MULTIMEDIA</t>
+        </is>
+      </c>
+      <c r="D31" s="6" t="inlineStr">
+        <is>
+          <t>Negociación, Marketing Digital</t>
+        </is>
+      </c>
+      <c r="E31" s="6" t="inlineStr">
+        <is>
+          <t>Realizar negociación con los proveedores y clientes, según los objetivos y estrategias establecidas por la organización.</t>
+        </is>
+      </c>
+      <c r="F31" s="6" t="inlineStr">
+        <is>
+          <t>Realizar negociación con los proveedores y clientes, según los objetivos y estrategias establecidas por la organización.</t>
+        </is>
+      </c>
+      <c r="G31" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Definir el costo del proyecto teniendo en cuenta los gastos fijos, variables y tiempo invertido en la realización del mismo. </t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="6" t="inlineStr">
         <is>
           <t>2651969 A</t>
         </is>
       </c>
-      <c r="B29" s="6" t="n">
+      <c r="B32" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="C29" s="6" t="inlineStr">
+      <c r="C32" s="6" t="inlineStr">
         <is>
           <t>MULTIMEDIA</t>
         </is>
       </c>
-      <c r="D29" s="6" t="inlineStr">
+      <c r="D32" s="6" t="inlineStr">
         <is>
           <t>Proyecto (pruebas de usuario)</t>
         </is>
       </c>
-      <c r="E29" s="6" t="inlineStr">
+      <c r="E32" s="6" t="inlineStr">
         <is>
           <t>Entregar la aplicación multimedia para evaluar la satisfacción del cliente</t>
         </is>
       </c>
-      <c r="F29" s="6" t="inlineStr">
+      <c r="F32" s="6" t="inlineStr">
         <is>
           <t>Entregar la aplicación multimedia para evaluar la satisfacción del cliente</t>
         </is>
       </c>
-      <c r="G29" s="6" t="inlineStr">
+      <c r="G32" s="6" t="inlineStr">
         <is>
           <t>Realizar el empaque y los elementos de merchandising con los que se distribuirá el proyecto multimedia.</t>
         </is>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="6" t="inlineStr">
+    <row r="33">
+      <c r="A33" s="6" t="inlineStr"/>
+      <c r="B33" s="6" t="inlineStr"/>
+      <c r="C33" s="6" t="inlineStr">
+        <is>
+          <t>MULTIMEDIA</t>
+        </is>
+      </c>
+      <c r="D33" s="6" t="inlineStr">
+        <is>
+          <t>Proyecto (pruebas de usuario)</t>
+        </is>
+      </c>
+      <c r="E33" s="6" t="inlineStr">
+        <is>
+          <t>Entregar la aplicación multimedia para evaluar la satisfacción del cliente</t>
+        </is>
+      </c>
+      <c r="F33" s="6" t="inlineStr">
+        <is>
+          <t>Entregar la aplicación multimedia para evaluar la satisfacción del cliente</t>
+        </is>
+      </c>
+      <c r="G33" s="6" t="inlineStr">
+        <is>
+          <t>Realizar las modificaciones pertinentes de acuerdo con lo evaluado en las pruebas de accesibilidad, diseño, escalabilidad y usabilidad de la multimedia.</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="6" t="inlineStr"/>
+      <c r="B34" s="6" t="inlineStr"/>
+      <c r="C34" s="6" t="inlineStr">
+        <is>
+          <t>MULTIMEDIA</t>
+        </is>
+      </c>
+      <c r="D34" s="6" t="inlineStr">
+        <is>
+          <t>Proyecto (pruebas de usuario)</t>
+        </is>
+      </c>
+      <c r="E34" s="6" t="inlineStr">
+        <is>
+          <t>Entregar la aplicación multimedia para evaluar la satisfacción del cliente</t>
+        </is>
+      </c>
+      <c r="F34" s="6" t="inlineStr">
+        <is>
+          <t>Entregar la aplicación multimedia para evaluar la satisfacción del cliente</t>
+        </is>
+      </c>
+      <c r="G34" s="6" t="inlineStr">
+        <is>
+          <t>Elaborar los manuales y ayudas análogas o digitales necesarias para facilitar la operación del proyecto multimedia.</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="6" t="inlineStr">
         <is>
           <t>2771153 A</t>
         </is>
       </c>
-      <c r="B30" s="6" t="n">
+      <c r="B35" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="C30" s="6" t="inlineStr">
+      <c r="C35" s="6" t="inlineStr">
         <is>
           <t>INT CONT DIGITALES</t>
         </is>
       </c>
-      <c r="D30" s="6" t="inlineStr">
+      <c r="D35" s="6" t="inlineStr">
         <is>
           <t>Marketing Digital</t>
         </is>
       </c>
-      <c r="E30" s="6" t="inlineStr">
+      <c r="E35" s="6" t="inlineStr">
         <is>
           <t>Animar el contenido de acuerdo con técnicas y proyecto audiovisual</t>
         </is>
       </c>
-      <c r="F30" s="6" t="inlineStr">
+      <c r="F35" s="6" t="inlineStr">
         <is>
           <t>Elaborar las animaciones para la estrategia digital.</t>
         </is>
       </c>
-      <c r="G30" s="6" t="inlineStr">
+      <c r="G35" s="6" t="inlineStr">
         <is>
           <t>Verificar la estrategia digital de acuerdo con el guion.</t>
         </is>

</xml_diff>